<commit_message>
Affectation Preview Done !
</commit_message>
<xml_diff>
--- a/FusionDonnee.xlsx
+++ b/FusionDonnee.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7388" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7388" uniqueCount="800">
   <si>
     <t>Type Enseignant</t>
   </si>
@@ -2412,6 +2412,9 @@
   </si>
   <si>
     <t xml:space="preserve">5354 : Gestion de projets </t>
+  </si>
+  <si>
+    <t>2412:Mémoire</t>
   </si>
 </sst>
 </file>
@@ -2755,8 +2758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A962" workbookViewId="0">
-      <selection activeCell="G987" sqref="G987"/>
+    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
+      <selection activeCell="G333" sqref="G333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13594,7 +13597,7 @@
         <v>284</v>
       </c>
       <c r="G333" s="1" t="s">
-        <v>337</v>
+        <v>799</v>
       </c>
       <c r="J333" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Revert "Affectation Preview Done !"
This reverts commit 327995b0330c92fd7e854622ca6935b67e8b670b.
</commit_message>
<xml_diff>
--- a/FusionDonnee.xlsx
+++ b/FusionDonnee.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7388" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7388" uniqueCount="799">
   <si>
     <t>Type Enseignant</t>
   </si>
@@ -2412,9 +2412,6 @@
   </si>
   <si>
     <t xml:space="preserve">5354 : Gestion de projets </t>
-  </si>
-  <si>
-    <t>2412:Mémoire</t>
   </si>
 </sst>
 </file>
@@ -2758,8 +2755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
-      <selection activeCell="G333" sqref="G333"/>
+    <sheetView tabSelected="1" topLeftCell="A962" workbookViewId="0">
+      <selection activeCell="G987" sqref="G987"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13597,7 +13594,7 @@
         <v>284</v>
       </c>
       <c r="G333" s="1" t="s">
-        <v>799</v>
+        <v>337</v>
       </c>
       <c r="J333" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Affecation Preview Done !
</commit_message>
<xml_diff>
--- a/FusionDonnee.xlsx
+++ b/FusionDonnee.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7388" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7388" uniqueCount="800">
   <si>
     <t>Type Enseignant</t>
   </si>
@@ -2412,6 +2412,9 @@
   </si>
   <si>
     <t xml:space="preserve">5354 : Gestion de projets </t>
+  </si>
+  <si>
+    <t>2412:Mémoire</t>
   </si>
 </sst>
 </file>
@@ -2755,8 +2758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A962" workbookViewId="0">
-      <selection activeCell="G987" sqref="G987"/>
+    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
+      <selection activeCell="G333" sqref="G333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13594,7 +13597,7 @@
         <v>284</v>
       </c>
       <c r="G333" s="1" t="s">
-        <v>337</v>
+        <v>799</v>
       </c>
       <c r="J333" s="1">
         <v>0</v>

</xml_diff>